<commit_message>
pull down bij base van bjt
</commit_message>
<xml_diff>
--- a/Circuit/Bill Of Materials/BOM.xlsx
+++ b/Circuit/Bill Of Materials/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufp\Desktop\School\ProjectEmbedded\Workshop-IOT-RPI-2022-23\Circuit\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4615E6F-0E20-47A8-AA2B-310D6D7FF5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3786E2-A031-4A7E-9CDF-8093B7E6C68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{586D246B-09C9-41AC-BF81-1593AEFBAA71}"/>
+    <workbookView xWindow="14700" yWindow="4032" windowWidth="17280" windowHeight="8964" xr2:uid="{586D246B-09C9-41AC-BF81-1593AEFBAA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>DHT-11</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>910 ohm</t>
+  </si>
+  <si>
+    <t>Rauf</t>
+  </si>
+  <si>
+    <t>Hebben we?</t>
+  </si>
+  <si>
+    <t>RPI header</t>
+  </si>
+  <si>
+    <t>2x20</t>
   </si>
 </sst>
 </file>
@@ -513,19 +525,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED99C29-B4FE-4D84-B5A0-514B4AA5A6C0}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="158.7109375" customWidth="1"/>
+    <col min="1" max="3" width="33.88671875" customWidth="1"/>
+    <col min="4" max="4" width="158.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -539,7 +551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -553,7 +565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -564,10 +576,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -581,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -595,7 +607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -609,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -623,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -637,7 +649,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -647,11 +659,11 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -659,6 +671,20 @@
         <v>24</v>
       </c>
       <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>